<commit_message>
Desenvolvimento do relatório. Exercício 3 finalizado.
</commit_message>
<xml_diff>
--- a/TP2/Ex3.xlsx
+++ b/TP2/Ex3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Codificador</t>
   </si>
@@ -44,10 +44,52 @@
     <t>apostadores.txt</t>
   </si>
   <si>
-    <t>Winrar</t>
-  </si>
-  <si>
-    <t>7-Zip</t>
+    <t>Codificador/Método</t>
+  </si>
+  <si>
+    <t>Winrar - Dicionário 64KB</t>
+  </si>
+  <si>
+    <t>Winrar - Dicionário 4096KB</t>
+  </si>
+  <si>
+    <t>7-Zip - LZMA2, Dic 16MB</t>
+  </si>
+  <si>
+    <t>Winrar - Dic 64KB</t>
+  </si>
+  <si>
+    <t>Winrar - Dic 4096KB</t>
+  </si>
+  <si>
+    <t>7-Zip - PPMd</t>
+  </si>
+  <si>
+    <t>7-Zip - LZMA</t>
+  </si>
+  <si>
+    <t>7-Zip - LZMA2</t>
+  </si>
+  <si>
+    <t>7-Zip - BZip2</t>
+  </si>
+  <si>
+    <t>Número de Entradas</t>
+  </si>
+  <si>
+    <t>Ficheiro Original</t>
+  </si>
+  <si>
+    <t>Ficheiro Comprimido</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^4</t>
+  </si>
+  <si>
+    <t>10^5</t>
   </si>
 </sst>
 </file>
@@ -213,14 +255,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -230,24 +272,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
@@ -255,6 +284,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -264,9 +303,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -584,150 +640,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:C10"/>
+      <selection activeCell="I10" sqref="F1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="3">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="2">
         <v>28079</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>99626</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="F1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="F2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="7">
         <v>7762</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="8">
         <f>B3/D1</f>
         <v>0.27643434595249117</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="F3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7">
+        <v>28079</v>
+      </c>
+      <c r="H3" s="9">
+        <v>5768</v>
+      </c>
+      <c r="I3" s="8">
+        <f>H3/G3</f>
+        <v>0.20542042095516222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7">
         <v>7864</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="8">
         <f>B4/D1</f>
         <v>0.28006695395135156</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="F4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="7">
+        <v>280629</v>
+      </c>
+      <c r="H4" s="25">
+        <v>51411</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" ref="I4:I5" si="0">H4/G4</f>
+        <v>0.18319917043498712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="7">
+        <v>7864</v>
+      </c>
+      <c r="C5" s="8">
+        <f>B5/D1</f>
+        <v>0.28006695395135156</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2906959</v>
+      </c>
+      <c r="H5" s="25">
+        <v>542999</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18679279618322792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7">
         <v>6800</v>
       </c>
-      <c r="C5" s="13">
-        <f>B5/D1</f>
+      <c r="C6" s="8">
+        <f>B6/D1</f>
         <v>0.24217386659069054</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="F6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9">
+        <v>6793</v>
+      </c>
+      <c r="C7" s="8">
+        <f>B7/D1</f>
+        <v>0.24192456996331779</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>5768</v>
+      </c>
+      <c r="C8" s="8">
+        <f>B8/D1</f>
+        <v>0.20542042095516222</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7">
+        <v>99626</v>
+      </c>
+      <c r="H8" s="9">
+        <v>24097</v>
+      </c>
+      <c r="I8" s="8">
+        <f>H8/G8</f>
+        <v>0.24187461104530947</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9">
+        <v>5803</v>
+      </c>
+      <c r="C9" s="8">
+        <f>B9/D1</f>
+        <v>0.20666690409202607</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7">
+        <v>990470</v>
+      </c>
+      <c r="H9" s="25">
+        <v>178409</v>
+      </c>
+      <c r="I9" s="8">
+        <f>H9/G9</f>
+        <v>0.18012559693882702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="F10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="19">
+        <v>9905460</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1603825</v>
+      </c>
+      <c r="I10" s="8">
+        <f>H10/G10</f>
+        <v>0.16191322765424321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B12" s="7">
         <v>34614</v>
       </c>
-      <c r="C8" s="13">
-        <f>B8/E1</f>
+      <c r="C12" s="8">
+        <f>B12/E1</f>
         <v>0.34743942344367934</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="12">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
         <v>32397</v>
       </c>
-      <c r="C9" s="13">
-        <f>B9/E1</f>
+      <c r="C13" s="8">
+        <f>B13/E1</f>
         <v>0.32518619637444041</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="18">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="19">
+        <v>32744</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B14/E1</f>
+        <v>0.32866922289362216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
         <v>28652</v>
       </c>
-      <c r="C10" s="19">
-        <f>B10/E1</f>
+      <c r="C15" s="8">
+        <f>B15/E1</f>
         <v>0.2875956075723205</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9">
+        <v>28645</v>
+      </c>
+      <c r="C16" s="8">
+        <f>B16/E1</f>
+        <v>0.2875253447895128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9">
+        <v>24097</v>
+      </c>
+      <c r="C17" s="8">
+        <f>B17/E1</f>
+        <v>0.24187461104530947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9">
+        <v>25903</v>
+      </c>
+      <c r="C18" s="8">
+        <f>B18/E1</f>
+        <v>0.26000240900969629</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>